<commit_message>
Added another API viewport
- New small API viewport for future mini-map
- More file reorganization
</commit_message>
<xml_diff>
--- a/DirectX11 Level Renderer/DirectX11/docs/Project Rubric.xlsx
+++ b/DirectX11 Level Renderer/DirectX11/docs/Project Rubric.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e87c385a0523d84e/Documents/Full Sail/3D Content Creation/3dcc-course-materials-CodeWithJazmine/Assignment 2/DirectX11/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e87c385a0523d84e/Desktop/DirectX-11-Level-Renderer/DirectX11 Level Renderer/DirectX11/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="176" documentId="13_ncr:1_{3BA54DA0-33D1-42D2-A2A2-AD35B96A3236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3E4E466-9BC6-4EF8-AC67-81CB288C3794}"/>
   <bookViews>
-    <workbookView xWindow="13140" yWindow="930" windowWidth="21315" windowHeight="18090" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
+    <workbookView xWindow="-1830" yWindow="1050" windowWidth="21315" windowHeight="18090" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2061,10 +2061,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -2365,7 +2361,7 @@
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>